<commit_message>
add new exercises, definitions, update decks/wordlists
- updated anki decks/wordlists for Lesson 11. (3rd ed.)
- added new definitions to the dictionary.
- added the following exercises.

# Lesson 11 (3rd ed.)
- Kanji Vocabulary: 手, 紙, and 好
- Kanji Vocabulary: 近, 明, 病, and 院
- Kanji Vocabulary: 映, 画, and 歌
- Kanji Vocabulary: 市, 所, and 勉
- Kanji Vocabulary: 強, 有, and 旅
- Kanji Practice: Compounds
</commit_message>
<xml_diff>
--- a/resources/tools/wordlist_E-J/lessons-3rd/lesson-11.xlsx
+++ b/resources/tools/wordlist_E-J/lessons-3rd/lesson-11.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B99"/>
+  <dimension ref="A1:B164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1609,6 +1609,786 @@
         </is>
       </c>
     </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>letter</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>手紙|てがみ</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>singer</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>歌手|かしゅ</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>hand</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>手|て</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>sign language</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>手話|しゅわ</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>good at</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>上手な|じょうずな</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>paper</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>紙|かみ</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Japanese paper</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>和紙|わし</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>cover page</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>表紙|ひょうし</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>origami</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>折り紙|おりがみ</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>to like</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>好きな|すきな</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>to love</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>大好きな|だいすきな</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>goodwill</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>好意|こうい</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>liking; taste</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>好み|このみ</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>favorite food</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>好物|こうぶつ</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>near; nearby</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>近く|ちかく</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>neighborhood</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>近所|きんじょ</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>recently</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>最近|さいきん</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>the Middle and Near East</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>中近東|ちゅうきんとう</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>cheerful; bright</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>明るい|あかるい</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>tomorrow</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>明日|あした</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>explanation</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>説明|せつめい</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>invention</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>発明|はつめい</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>civilization</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>文明|ぶんめい</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>hospital</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>病院|びょういん</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>illness</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>病気|びょうき</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>serious illness</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>重病|じゅうびょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>sudden illness</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>急病|きゅうびょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>graduate school</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>大学院|だいがくいん</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>beauty parlor</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>美容院|びよういん</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>movie</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>映画|えいが</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>movie theater</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>映画館|えいがかん</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>to be reflected</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>映る|うつる</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>painter</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>画家|がか</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>plan</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>計画|けいかく</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>comic</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>漫画|まんが</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>to sing</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>歌う|うたう</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>song</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>歌|うた</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>singer</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>歌手|かしゅ</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>national anthem</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>国歌|こっか</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Kabuki</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>歌舞伎|かぶき</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>lyrics</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>歌詞|かし</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Kawaguchi City</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>川口市|かわぐちし</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>city hall</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>市役所|しやくしょ</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>mayor</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>市長|しちょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>market</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>市場|いちば</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>various places</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>いろいろな所|いろいろなところ</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>neighborhood</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>近所|きんじょ</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>kitchen</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>台所|だいどころ</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>address</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>住所|じゅうしょ</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>to study</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>勉強する|べんきょうする</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>to try hard</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>勉める|つとめる</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>diligent</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>勤勉な|きんべんな</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>to study</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>勉強する|べんきょうする</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>strong</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>強い|つよい</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>obstinate</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>強情な|ごうじょうな</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>robbery</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>強盗|ごうとう</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>powerful</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>強力な|きょうりょくな</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>famous</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>有名な|ゆうめいな</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>toll; fee</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>有料|ゆうりょう</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>to exist</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>有る|ある</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>talented</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>有能な|ゆうのうな</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>travel</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>旅行|りょこう</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Japanese inn</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>旅館|りょかん</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>traveling alone</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>一人旅|ひとりたび</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>passport</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>旅券|りょけん</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>